<commit_message>
Mejora guia y enlaces catalogo
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2a9e946ecd1f9e6/DNP - Guía de buenas practicas Genero - IA/Seguimiento técnico -contrato 1104-2024 DNP/Entregables/Entregable 3/Árbol de decisión/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{D4A6E784-F98D-4FAC-A4C6-E98783F1CD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7D2AB24-A3A5-4A13-849E-D7D20B031386}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{D4A6E784-F98D-4FAC-A4C6-E98783F1CD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93E98A7C-07CB-4F8F-8553-22BDEB2CD0D9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guía" sheetId="11" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="628">
   <si>
     <t>ID</t>
   </si>
@@ -2920,6 +2920,9 @@
   </si>
   <si>
     <t>Mantener la medida xx</t>
+  </si>
+  <si>
+    <t>URL</t>
   </si>
 </sst>
 </file>
@@ -3765,18 +3768,18 @@
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="55"/>
-    <col min="2" max="2" width="22.28515625" style="55" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="55"/>
+    <col min="2" max="2" width="22.33203125" style="55" customWidth="1"/>
     <col min="3" max="3" width="29" style="55" customWidth="1"/>
-    <col min="4" max="5" width="93.42578125" style="55" customWidth="1"/>
+    <col min="4" max="5" width="93.44140625" style="55" customWidth="1"/>
     <col min="6" max="6" width="23" style="55" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="55" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="55"/>
+    <col min="7" max="7" width="29.44140625" style="55" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="60" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="60" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
@@ -3799,7 +3802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>6</v>
       </c>
@@ -3822,7 +3825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
         <v>13</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56" t="s">
         <v>16</v>
       </c>
@@ -3868,7 +3871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
         <v>20</v>
       </c>
@@ -3891,7 +3894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56" t="s">
         <v>23</v>
       </c>
@@ -3914,7 +3917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
         <v>27</v>
       </c>
@@ -3937,7 +3940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56" t="s">
         <v>32</v>
       </c>
@@ -3960,7 +3963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56" t="s">
         <v>35</v>
       </c>
@@ -3983,7 +3986,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="56" t="s">
         <v>38</v>
       </c>
@@ -4006,7 +4009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="56" t="s">
         <v>41</v>
       </c>
@@ -4029,7 +4032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="56" t="s">
         <v>45</v>
       </c>
@@ -4052,7 +4055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="56" t="s">
         <v>49</v>
       </c>
@@ -4075,7 +4078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="56" t="s">
         <v>53</v>
       </c>
@@ -4098,7 +4101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="56" t="s">
         <v>57</v>
       </c>
@@ -4121,7 +4124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="56" t="s">
         <v>60</v>
       </c>
@@ -4144,7 +4147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="56" t="s">
         <v>63</v>
       </c>
@@ -4167,7 +4170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="56" t="s">
         <v>67</v>
       </c>
@@ -4190,7 +4193,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="56" t="s">
         <v>70</v>
       </c>
@@ -4213,7 +4216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="56" t="s">
         <v>74</v>
       </c>
@@ -4236,7 +4239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="56" t="s">
         <v>77</v>
       </c>
@@ -4259,7 +4262,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="56" t="s">
         <v>81</v>
       </c>
@@ -4282,7 +4285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="56" t="s">
         <v>84</v>
       </c>
@@ -4305,7 +4308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="56" t="s">
         <v>87</v>
       </c>
@@ -4328,7 +4331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="56" t="s">
         <v>6</v>
       </c>
@@ -4349,7 +4352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="56" t="s">
         <v>13</v>
       </c>
@@ -4370,7 +4373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="56" t="s">
         <v>16</v>
       </c>
@@ -4391,7 +4394,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="56" t="s">
         <v>20</v>
       </c>
@@ -4412,7 +4415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="56" t="s">
         <v>23</v>
       </c>
@@ -4447,26 +4450,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="249.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="249.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="4" width="18.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="4" width="18.5546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="65" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="26" style="2" customWidth="1"/>
-    <col min="8" max="8" width="52.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="52.88671875" style="2" customWidth="1"/>
     <col min="9" max="9" width="23" style="2" customWidth="1"/>
-    <col min="10" max="10" width="32.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="34.140625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="10" width="32.44140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="34.109375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>102</v>
       </c>
@@ -4492,13 +4495,13 @@
         <v>109</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>110</v>
+        <v>627</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="138" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -4530,7 +4533,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="183.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -4562,7 +4565,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -4594,7 +4597,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="296.10000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="296.10000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -4626,7 +4629,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="216.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="216.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -4658,7 +4661,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="207.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="207.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -4691,7 +4694,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="201" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="201" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -4723,7 +4726,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="257.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -4755,7 +4758,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="271.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="271.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -4787,7 +4790,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="228.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="228.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -4819,7 +4822,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="191.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="191.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -4851,7 +4854,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="172.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -4883,7 +4886,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -4915,7 +4918,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -4947,7 +4950,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -4979,7 +4982,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -5012,7 +5015,7 @@
       </c>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -5044,7 +5047,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -5076,7 +5079,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -5108,7 +5111,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -5140,19 +5143,19 @@
         <v>269</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
@@ -5213,14 +5216,14 @@
       <selection pane="bottomLeft" activeCell="A45" sqref="A45:A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="81" style="7" customWidth="1"/>
     <col min="2" max="2" width="53" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>103</v>
       </c>
@@ -5228,7 +5231,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>112</v>
       </c>
@@ -5236,7 +5239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>112</v>
       </c>
@@ -5244,7 +5247,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>112</v>
       </c>
@@ -5252,7 +5255,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>112</v>
       </c>
@@ -5260,7 +5263,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>121</v>
       </c>
@@ -5268,7 +5271,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>121</v>
       </c>
@@ -5276,7 +5279,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>121</v>
       </c>
@@ -5284,7 +5287,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>130</v>
       </c>
@@ -5292,7 +5295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>130</v>
       </c>
@@ -5300,7 +5303,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>130</v>
       </c>
@@ -5308,7 +5311,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>130</v>
       </c>
@@ -5316,7 +5319,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>137</v>
       </c>
@@ -5324,7 +5327,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>137</v>
       </c>
@@ -5332,7 +5335,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>154</v>
       </c>
@@ -5340,7 +5343,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>154</v>
       </c>
@@ -5348,7 +5351,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>154</v>
       </c>
@@ -5356,7 +5359,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>145</v>
       </c>
@@ -5364,7 +5367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>145</v>
       </c>
@@ -5372,7 +5375,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>161</v>
       </c>
@@ -5380,7 +5383,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>161</v>
       </c>
@@ -5388,7 +5391,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>168</v>
       </c>
@@ -5396,7 +5399,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>168</v>
       </c>
@@ -5404,7 +5407,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>168</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>168</v>
       </c>
@@ -5420,7 +5423,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>168</v>
       </c>
@@ -5428,7 +5431,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>177</v>
       </c>
@@ -5436,7 +5439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>177</v>
       </c>
@@ -5444,7 +5447,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>177</v>
       </c>
@@ -5452,7 +5455,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>177</v>
       </c>
@@ -5460,7 +5463,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>191</v>
       </c>
@@ -5468,7 +5471,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>191</v>
       </c>
@@ -5476,7 +5479,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>191</v>
       </c>
@@ -5484,7 +5487,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>198</v>
       </c>
@@ -5492,7 +5495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>198</v>
       </c>
@@ -5500,7 +5503,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>198</v>
       </c>
@@ -5508,7 +5511,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>198</v>
       </c>
@@ -5516,7 +5519,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>198</v>
       </c>
@@ -5524,7 +5527,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>206</v>
       </c>
@@ -5532,7 +5535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>206</v>
       </c>
@@ -5540,7 +5543,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>206</v>
       </c>
@@ -5548,7 +5551,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>214</v>
       </c>
@@ -5556,7 +5559,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>223</v>
       </c>
@@ -5564,7 +5567,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>223</v>
       </c>
@@ -5572,7 +5575,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>231</v>
       </c>
@@ -5580,7 +5583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>231</v>
       </c>
@@ -5588,7 +5591,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>231</v>
       </c>
@@ -5596,7 +5599,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>231</v>
       </c>
@@ -5604,7 +5607,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>272</v>
       </c>
@@ -5612,7 +5615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>272</v>
       </c>
@@ -5620,7 +5623,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>272</v>
       </c>
@@ -5628,7 +5631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>238</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>238</v>
       </c>
@@ -5644,7 +5647,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>246</v>
       </c>
@@ -5652,7 +5655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>246</v>
       </c>
@@ -5660,7 +5663,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>254</v>
       </c>
@@ -5668,7 +5671,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>254</v>
       </c>
@@ -5676,7 +5679,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>262</v>
       </c>
@@ -5684,67 +5687,67 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
     </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
     </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
     </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
     </row>
-    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
     </row>
-    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
     </row>
-    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
     </row>
-    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
     </row>
-    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
     </row>
-    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
     </row>
-    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
     </row>
@@ -5781,14 +5784,14 @@
       <selection pane="bottomLeft" activeCell="A65" sqref="A65:A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" style="7" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="2" max="2" width="47.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>103</v>
       </c>
@@ -5796,7 +5799,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>112</v>
       </c>
@@ -5804,7 +5807,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>112</v>
       </c>
@@ -5812,7 +5815,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>112</v>
       </c>
@@ -5820,7 +5823,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>112</v>
       </c>
@@ -5828,7 +5831,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>112</v>
       </c>
@@ -5836,7 +5839,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>112</v>
       </c>
@@ -5844,7 +5847,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>121</v>
       </c>
@@ -5852,7 +5855,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>121</v>
       </c>
@@ -5860,7 +5863,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -5868,7 +5871,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>121</v>
       </c>
@@ -5876,7 +5879,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>130</v>
       </c>
@@ -5884,7 +5887,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>130</v>
       </c>
@@ -5892,7 +5895,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>130</v>
       </c>
@@ -5900,7 +5903,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>130</v>
       </c>
@@ -5908,7 +5911,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>137</v>
       </c>
@@ -5916,7 +5919,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>137</v>
       </c>
@@ -5924,7 +5927,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>137</v>
       </c>
@@ -5932,7 +5935,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>137</v>
       </c>
@@ -5940,7 +5943,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>145</v>
       </c>
@@ -5948,7 +5951,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>145</v>
       </c>
@@ -5956,7 +5959,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>145</v>
       </c>
@@ -5964,7 +5967,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>145</v>
       </c>
@@ -5972,7 +5975,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>154</v>
       </c>
@@ -5980,7 +5983,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>154</v>
       </c>
@@ -5988,7 +5991,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>154</v>
       </c>
@@ -5996,7 +5999,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>154</v>
       </c>
@@ -6004,7 +6007,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>154</v>
       </c>
@@ -6012,7 +6015,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>161</v>
       </c>
@@ -6020,7 +6023,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>161</v>
       </c>
@@ -6028,7 +6031,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>161</v>
       </c>
@@ -6036,7 +6039,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>161</v>
       </c>
@@ -6044,7 +6047,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>161</v>
       </c>
@@ -6052,7 +6055,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>161</v>
       </c>
@@ -6060,7 +6063,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>161</v>
       </c>
@@ -6068,7 +6071,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>168</v>
       </c>
@@ -6076,7 +6079,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>168</v>
       </c>
@@ -6084,7 +6087,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>168</v>
       </c>
@@ -6092,7 +6095,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>168</v>
       </c>
@@ -6100,7 +6103,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>168</v>
       </c>
@@ -6108,7 +6111,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>177</v>
       </c>
@@ -6116,7 +6119,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>177</v>
       </c>
@@ -6124,7 +6127,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>177</v>
       </c>
@@ -6132,7 +6135,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>177</v>
       </c>
@@ -6140,7 +6143,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>185</v>
       </c>
@@ -6148,7 +6151,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>185</v>
       </c>
@@ -6156,7 +6159,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>185</v>
       </c>
@@ -6164,7 +6167,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>191</v>
       </c>
@@ -6172,7 +6175,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>191</v>
       </c>
@@ -6180,7 +6183,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>191</v>
       </c>
@@ -6188,7 +6191,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>198</v>
       </c>
@@ -6196,7 +6199,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>198</v>
       </c>
@@ -6204,7 +6207,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>198</v>
       </c>
@@ -6212,7 +6215,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>206</v>
       </c>
@@ -6220,7 +6223,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>206</v>
       </c>
@@ -6228,7 +6231,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>206</v>
       </c>
@@ -6236,7 +6239,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>206</v>
       </c>
@@ -6244,7 +6247,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>206</v>
       </c>
@@ -6252,7 +6255,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>214</v>
       </c>
@@ -6260,7 +6263,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>214</v>
       </c>
@@ -6268,7 +6271,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>214</v>
       </c>
@@ -6276,7 +6279,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>223</v>
       </c>
@@ -6284,7 +6287,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>223</v>
       </c>
@@ -6292,7 +6295,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>223</v>
       </c>
@@ -6300,7 +6303,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>231</v>
       </c>
@@ -6308,7 +6311,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>231</v>
       </c>
@@ -6316,7 +6319,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>231</v>
       </c>
@@ -6324,7 +6327,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>231</v>
       </c>
@@ -6332,7 +6335,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>231</v>
       </c>
@@ -6340,7 +6343,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>231</v>
       </c>
@@ -6348,7 +6351,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>231</v>
       </c>
@@ -6356,7 +6359,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>272</v>
       </c>
@@ -6364,7 +6367,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>272</v>
       </c>
@@ -6372,7 +6375,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>272</v>
       </c>
@@ -6380,7 +6383,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>238</v>
       </c>
@@ -6388,7 +6391,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>238</v>
       </c>
@@ -6396,7 +6399,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>238</v>
       </c>
@@ -6404,7 +6407,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>238</v>
       </c>
@@ -6412,7 +6415,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>238</v>
       </c>
@@ -6420,7 +6423,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>246</v>
       </c>
@@ -6428,7 +6431,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>246</v>
       </c>
@@ -6436,7 +6439,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>246</v>
       </c>
@@ -6444,7 +6447,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>254</v>
       </c>
@@ -6452,7 +6455,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>254</v>
       </c>
@@ -6460,7 +6463,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>254</v>
       </c>
@@ -6468,7 +6471,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>254</v>
       </c>
@@ -6476,7 +6479,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>262</v>
       </c>
@@ -6484,7 +6487,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>262</v>
       </c>
@@ -6492,7 +6495,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>262</v>
       </c>
@@ -6500,23 +6503,23 @@
         <v>277</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
     </row>
-    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
     </row>
-    <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
     </row>
-    <row r="93" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
     </row>
-    <row r="94" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
     </row>
@@ -6553,14 +6556,14 @@
       <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="81" style="7" customWidth="1"/>
     <col min="2" max="2" width="53" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>103</v>
       </c>
@@ -6568,7 +6571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>112</v>
       </c>
@@ -6576,7 +6579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>112</v>
       </c>
@@ -6584,7 +6587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>112</v>
       </c>
@@ -6592,7 +6595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>121</v>
       </c>
@@ -6600,7 +6603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>121</v>
       </c>
@@ -6608,7 +6611,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>121</v>
       </c>
@@ -6616,7 +6619,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>130</v>
       </c>
@@ -6624,7 +6627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>130</v>
       </c>
@@ -6632,7 +6635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>137</v>
       </c>
@@ -6640,7 +6643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>145</v>
       </c>
@@ -6648,7 +6651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>154</v>
       </c>
@@ -6656,7 +6659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>161</v>
       </c>
@@ -6664,7 +6667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>168</v>
       </c>
@@ -6672,7 +6675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>168</v>
       </c>
@@ -6680,7 +6683,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>168</v>
       </c>
@@ -6688,7 +6691,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>177</v>
       </c>
@@ -6696,7 +6699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>185</v>
       </c>
@@ -6704,7 +6707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>191</v>
       </c>
@@ -6712,7 +6715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>191</v>
       </c>
@@ -6720,7 +6723,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>198</v>
       </c>
@@ -6728,7 +6731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>198</v>
       </c>
@@ -6736,7 +6739,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>198</v>
       </c>
@@ -6744,7 +6747,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>206</v>
       </c>
@@ -6752,7 +6755,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>214</v>
       </c>
@@ -6760,7 +6763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>223</v>
       </c>
@@ -6768,7 +6771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>231</v>
       </c>
@@ -6776,7 +6779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>231</v>
       </c>
@@ -6784,7 +6787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>272</v>
       </c>
@@ -6792,7 +6795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>272</v>
       </c>
@@ -6800,7 +6803,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>238</v>
       </c>
@@ -6808,7 +6811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>246</v>
       </c>
@@ -6816,7 +6819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>254</v>
       </c>
@@ -6824,7 +6827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>262</v>
       </c>
@@ -6865,14 +6868,14 @@
       <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="98.140625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="26.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="98.109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>281</v>
       </c>
@@ -6880,7 +6883,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>282</v>
       </c>
@@ -6888,7 +6891,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>106</v>
       </c>
@@ -6896,7 +6899,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>105</v>
       </c>
@@ -6904,7 +6907,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>104</v>
       </c>
@@ -6912,7 +6915,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>287</v>
       </c>
@@ -6920,7 +6923,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="38" t="s">
         <v>289</v>
       </c>
@@ -6928,7 +6931,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
         <v>291</v>
       </c>
@@ -6936,7 +6939,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
         <v>4</v>
       </c>
@@ -6944,7 +6947,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>294</v>
       </c>
@@ -6952,7 +6955,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>108</v>
       </c>
@@ -6960,7 +6963,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>297</v>
       </c>
@@ -6968,7 +6971,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>299</v>
       </c>
@@ -6976,7 +6979,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>301</v>
       </c>
@@ -6984,7 +6987,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>303</v>
       </c>
@@ -7001,25 +7004,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA93528-64C0-4424-AA74-D29A95719F58}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="26" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="41.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="34.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="41.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="36.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7045,7 +7048,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>307</v>
       </c>
@@ -7071,7 +7074,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>314</v>
       </c>
@@ -7097,7 +7100,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>319</v>
       </c>
@@ -7123,7 +7126,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>324</v>
       </c>
@@ -7149,7 +7152,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>329</v>
       </c>
@@ -7175,7 +7178,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>335</v>
       </c>
@@ -7201,7 +7204,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>339</v>
       </c>
@@ -7227,7 +7230,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>344</v>
       </c>
@@ -7253,7 +7256,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>349</v>
       </c>
@@ -7279,7 +7282,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>355</v>
       </c>
@@ -7305,7 +7308,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>360</v>
       </c>
@@ -7331,7 +7334,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>365</v>
       </c>
@@ -7357,7 +7360,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>370</v>
       </c>
@@ -7383,7 +7386,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>376</v>
       </c>
@@ -7409,7 +7412,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>380</v>
       </c>
@@ -7435,7 +7438,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>385</v>
       </c>
@@ -7461,7 +7464,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>390</v>
       </c>
@@ -7487,7 +7490,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>396</v>
       </c>
@@ -7513,7 +7516,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>401</v>
       </c>
@@ -7539,7 +7542,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>406</v>
       </c>
@@ -7565,7 +7568,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>411</v>
       </c>
@@ -7591,7 +7594,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>417</v>
       </c>
@@ -7617,7 +7620,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>422</v>
       </c>
@@ -7643,7 +7646,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>427</v>
       </c>
@@ -7669,7 +7672,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>432</v>
       </c>
@@ -7695,7 +7698,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>438</v>
       </c>
@@ -7721,7 +7724,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>443</v>
       </c>
@@ -7747,7 +7750,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>307</v>
       </c>
@@ -7773,7 +7776,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>314</v>
       </c>
@@ -7799,7 +7802,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>319</v>
       </c>
@@ -7825,7 +7828,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>324</v>
       </c>
@@ -7851,7 +7854,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>329</v>
       </c>
@@ -7877,7 +7880,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>335</v>
       </c>
@@ -7903,7 +7906,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>339</v>
       </c>
@@ -7929,7 +7932,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>344</v>
       </c>
@@ -7955,7 +7958,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>349</v>
       </c>
@@ -7981,7 +7984,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>355</v>
       </c>
@@ -8007,7 +8010,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>360</v>
       </c>
@@ -8033,7 +8036,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>365</v>
       </c>
@@ -8059,7 +8062,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>370</v>
       </c>
@@ -8085,7 +8088,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>376</v>
       </c>
@@ -8111,7 +8114,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -8121,7 +8124,7 @@
       <c r="G43"/>
       <c r="H43"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -8131,7 +8134,7 @@
       <c r="G44"/>
       <c r="H44"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -8141,7 +8144,7 @@
       <c r="G45"/>
       <c r="H45"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -8151,7 +8154,7 @@
       <c r="G46"/>
       <c r="H46"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -8175,18 +8178,18 @@
       <selection pane="bottomLeft" sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="59.5546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="59" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>523</v>
       </c>
@@ -8197,7 +8200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
@@ -8211,7 +8214,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>28</v>
       </c>
@@ -8225,7 +8228,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>271</v>
       </c>
@@ -8239,7 +8242,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>54</v>
       </c>
@@ -8248,7 +8251,7 @@
       </c>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>71</v>
       </c>
@@ -8257,7 +8260,7 @@
       </c>
       <c r="C6" s="10"/>
     </row>
-    <row r="7" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>78</v>
       </c>
@@ -8266,7 +8269,7 @@
       </c>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>528</v>
       </c>
@@ -8275,34 +8278,34 @@
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" ht="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="66.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="66.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="66.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8314,13 +8317,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="12" width="58.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="12" width="58.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>102</v>
       </c>
@@ -8356,7 +8359,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="180" x14ac:dyDescent="0.3">
       <c r="A2" s="26">
         <v>15</v>
       </c>
@@ -8394,7 +8397,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A3" s="26">
         <v>17</v>
       </c>
@@ -8432,7 +8435,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="196.2" x14ac:dyDescent="0.3">
       <c r="A4" s="26">
         <v>18</v>
       </c>
@@ -8470,7 +8473,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="285" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="285" x14ac:dyDescent="0.3">
       <c r="A5" s="26">
         <v>10</v>
       </c>
@@ -8506,7 +8509,7 @@
       </c>
       <c r="L5" s="31"/>
     </row>
-    <row r="6" spans="1:12" ht="240" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="240" x14ac:dyDescent="0.3">
       <c r="A6" s="37">
         <v>12</v>
       </c>
@@ -8544,7 +8547,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="195" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>13</v>
       </c>
@@ -8582,7 +8585,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="225" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>592</v>
       </c>
@@ -8620,7 +8623,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="195.6" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>16</v>
       </c>
@@ -8658,7 +8661,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>22</v>
       </c>

</xml_diff>